<commit_message>
Update sunny prize form.
</commit_message>
<xml_diff>
--- a/SMELuckyDraw/excel/namelist.xlsx
+++ b/SMELuckyDraw/excel/namelist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
   <si>
     <t>i076652</t>
   </si>
@@ -106,6 +106,42 @@
   </si>
   <si>
     <t>Zhang, SanC</t>
+  </si>
+  <si>
+    <t>Zhang, SanBD</t>
+  </si>
+  <si>
+    <t>Li, SiBd</t>
+  </si>
+  <si>
+    <t>Wang, WuBD</t>
+  </si>
+  <si>
+    <t>Zhou, LiuBD</t>
+  </si>
+  <si>
+    <t>Wu, QiBD</t>
+  </si>
+  <si>
+    <t>Zheng, BaBD</t>
+  </si>
+  <si>
+    <t>Zhang, SanCE</t>
+  </si>
+  <si>
+    <t>Li, SiCE</t>
+  </si>
+  <si>
+    <t>Wang, WuCE</t>
+  </si>
+  <si>
+    <t>Zhou, LiuCE</t>
+  </si>
+  <si>
+    <t>Wu, QiCE</t>
+  </si>
+  <si>
+    <t>Zheng, BaCE</t>
   </si>
 </sst>
 </file>
@@ -116,7 +152,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -145,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -161,7 +197,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -203,7 +239,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -238,7 +274,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,18 +483,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -474,7 +510,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -482,7 +518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -490,7 +526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -498,7 +534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -506,7 +542,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -514,7 +550,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -522,7 +558,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -530,7 +566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -538,7 +574,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -546,7 +582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -554,7 +590,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -562,7 +598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -570,7 +606,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -578,7 +614,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -586,7 +622,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -594,7 +630,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -602,7 +638,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -610,7 +646,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -618,7 +654,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -626,7 +662,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -634,7 +670,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -642,12 +678,108 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -661,7 +793,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -673,7 +805,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update project file, fix crash issue.
</commit_message>
<xml_diff>
--- a/SMELuckyDraw/excel/namelist.xlsx
+++ b/SMELuckyDraw/excel/namelist.xlsx
@@ -1312,9 +1312,6 @@
     <t>Xu, Anne</t>
   </si>
   <si>
-    <t>Han, Cun</t>
-  </si>
-  <si>
     <t>Liao, Henry</t>
   </si>
   <si>
@@ -1351,9 +1348,6 @@
     <t>Ke, Xianda</t>
   </si>
   <si>
-    <t>Xie, Fang Kai</t>
-  </si>
-  <si>
     <t>Shen,Qiuqiong</t>
   </si>
   <si>
@@ -1474,15 +1468,9 @@
     <t xml:space="preserve">Tang, Sara </t>
   </si>
   <si>
-    <t>Yifang Wang</t>
-  </si>
-  <si>
     <t>Chen, Doreen</t>
   </si>
   <si>
-    <t>Zhang,Yaotian</t>
-  </si>
-  <si>
     <t>Liu, Qing</t>
   </si>
   <si>
@@ -1705,9 +1693,6 @@
     <t>He, Huan</t>
   </si>
   <si>
-    <t>Wang, Yife</t>
-  </si>
-  <si>
     <t>Cui, Charlene</t>
   </si>
   <si>
@@ -1840,9 +1825,6 @@
     <t>Zhao, Ming</t>
   </si>
   <si>
-    <t>Dou, FeiFei</t>
-  </si>
-  <si>
     <t>Chen, Yun</t>
   </si>
   <si>
@@ -2240,6 +2222,24 @@
   </si>
   <si>
     <t>Sun, Wei</t>
+  </si>
+  <si>
+    <t>Wang, Yifei</t>
+  </si>
+  <si>
+    <t>Xie, Fangkai</t>
+  </si>
+  <si>
+    <t>Dou, Feifei</t>
+  </si>
+  <si>
+    <t>Zhang, Yaotian</t>
+  </si>
+  <si>
+    <t>Hang, Cun</t>
+  </si>
+  <si>
+    <t>Wang, Yifang</t>
   </si>
 </sst>
 </file>
@@ -2583,8 +2583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B372"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
+      <selection activeCell="B349" sqref="B349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2606,7 +2606,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2614,7 +2614,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2622,7 +2622,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2638,7 +2638,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2646,7 +2646,7 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2654,7 +2654,7 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>563</v>
+        <v>736</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2662,7 +2662,7 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2670,7 +2670,7 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2694,7 +2694,7 @@
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2766,7 +2766,7 @@
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2774,7 +2774,7 @@
         <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2782,7 +2782,7 @@
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2806,7 +2806,7 @@
         <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2838,7 +2838,7 @@
         <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2854,7 +2854,7 @@
         <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2862,7 +2862,7 @@
         <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2878,7 +2878,7 @@
         <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2910,7 +2910,7 @@
         <v>54</v>
       </c>
       <c r="B40" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2918,7 +2918,7 @@
         <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2934,7 +2934,7 @@
         <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2942,7 +2942,7 @@
         <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2950,7 +2950,7 @@
         <v>59</v>
       </c>
       <c r="B45" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2990,7 +2990,7 @@
         <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -3006,7 +3006,7 @@
         <v>66</v>
       </c>
       <c r="B52" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -3014,7 +3014,7 @@
         <v>67</v>
       </c>
       <c r="B53" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -3022,7 +3022,7 @@
         <v>68</v>
       </c>
       <c r="B54" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -3030,7 +3030,7 @@
         <v>69</v>
       </c>
       <c r="B55" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -3062,7 +3062,7 @@
         <v>73</v>
       </c>
       <c r="B59" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -3078,7 +3078,7 @@
         <v>75</v>
       </c>
       <c r="B61" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -3094,7 +3094,7 @@
         <v>77</v>
       </c>
       <c r="B63" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -3102,7 +3102,7 @@
         <v>78</v>
       </c>
       <c r="B64" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -3110,7 +3110,7 @@
         <v>79</v>
       </c>
       <c r="B65" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -3118,7 +3118,7 @@
         <v>80</v>
       </c>
       <c r="B66" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -3158,7 +3158,7 @@
         <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -3190,7 +3190,7 @@
         <v>89</v>
       </c>
       <c r="B75" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -3206,7 +3206,7 @@
         <v>91</v>
       </c>
       <c r="B77" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -3222,7 +3222,7 @@
         <v>93</v>
       </c>
       <c r="B79" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -3238,7 +3238,7 @@
         <v>95</v>
       </c>
       <c r="B81" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -3246,7 +3246,7 @@
         <v>96</v>
       </c>
       <c r="B82" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -3278,7 +3278,7 @@
         <v>100</v>
       </c>
       <c r="B86" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -3310,7 +3310,7 @@
         <v>104</v>
       </c>
       <c r="B90" t="s">
-        <v>432</v>
+        <v>740</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -3318,7 +3318,7 @@
         <v>105</v>
       </c>
       <c r="B91" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -3326,7 +3326,7 @@
         <v>106</v>
       </c>
       <c r="B92" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -3342,7 +3342,7 @@
         <v>108</v>
       </c>
       <c r="B94" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -3350,7 +3350,7 @@
         <v>109</v>
       </c>
       <c r="B95" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -3358,7 +3358,7 @@
         <v>110</v>
       </c>
       <c r="B96" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -3374,7 +3374,7 @@
         <v>112</v>
       </c>
       <c r="B98" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -3382,7 +3382,7 @@
         <v>113</v>
       </c>
       <c r="B99" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -3390,7 +3390,7 @@
         <v>114</v>
       </c>
       <c r="B100" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -3398,7 +3398,7 @@
         <v>115</v>
       </c>
       <c r="B101" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -3406,7 +3406,7 @@
         <v>116</v>
       </c>
       <c r="B102" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -3414,7 +3414,7 @@
         <v>117</v>
       </c>
       <c r="B103" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -3422,7 +3422,7 @@
         <v>118</v>
       </c>
       <c r="B104" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -3430,7 +3430,7 @@
         <v>119</v>
       </c>
       <c r="B105" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -3438,7 +3438,7 @@
         <v>120</v>
       </c>
       <c r="B106" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -3446,7 +3446,7 @@
         <v>121</v>
       </c>
       <c r="B107" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -3454,7 +3454,7 @@
         <v>122</v>
       </c>
       <c r="B108" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -3462,7 +3462,7 @@
         <v>123</v>
       </c>
       <c r="B109" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -3470,7 +3470,7 @@
         <v>124</v>
       </c>
       <c r="B110" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -3478,7 +3478,7 @@
         <v>125</v>
       </c>
       <c r="B111" t="s">
-        <v>445</v>
+        <v>737</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -3486,7 +3486,7 @@
         <v>126</v>
       </c>
       <c r="B112" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -3494,7 +3494,7 @@
         <v>127</v>
       </c>
       <c r="B113" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -3502,7 +3502,7 @@
         <v>128</v>
       </c>
       <c r="B114" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -3510,7 +3510,7 @@
         <v>129</v>
       </c>
       <c r="B115" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -3518,7 +3518,7 @@
         <v>130</v>
       </c>
       <c r="B116" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -3526,7 +3526,7 @@
         <v>131</v>
       </c>
       <c r="B117" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -3534,7 +3534,7 @@
         <v>132</v>
       </c>
       <c r="B118" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -3542,7 +3542,7 @@
         <v>133</v>
       </c>
       <c r="B119" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -3550,7 +3550,7 @@
         <v>134</v>
       </c>
       <c r="B120" t="s">
-        <v>608</v>
+        <v>738</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -3558,7 +3558,7 @@
         <v>135</v>
       </c>
       <c r="B121" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -3566,7 +3566,7 @@
         <v>136</v>
       </c>
       <c r="B122" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -3574,7 +3574,7 @@
         <v>137</v>
       </c>
       <c r="B123" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -3582,7 +3582,7 @@
         <v>138</v>
       </c>
       <c r="B124" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -3590,7 +3590,7 @@
         <v>139</v>
       </c>
       <c r="B125" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -3598,7 +3598,7 @@
         <v>140</v>
       </c>
       <c r="B126" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -3606,7 +3606,7 @@
         <v>141</v>
       </c>
       <c r="B127" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -3614,7 +3614,7 @@
         <v>142</v>
       </c>
       <c r="B128" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -3622,7 +3622,7 @@
         <v>143</v>
       </c>
       <c r="B129" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -3630,7 +3630,7 @@
         <v>144</v>
       </c>
       <c r="B130" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -3638,7 +3638,7 @@
         <v>145</v>
       </c>
       <c r="B131" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -3646,7 +3646,7 @@
         <v>146</v>
       </c>
       <c r="B132" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -3654,7 +3654,7 @@
         <v>147</v>
       </c>
       <c r="B133" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -3662,7 +3662,7 @@
         <v>148</v>
       </c>
       <c r="B134" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -3670,7 +3670,7 @@
         <v>149</v>
       </c>
       <c r="B135" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -3678,7 +3678,7 @@
         <v>150</v>
       </c>
       <c r="B136" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -3694,7 +3694,7 @@
         <v>152</v>
       </c>
       <c r="B138" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -3702,7 +3702,7 @@
         <v>153</v>
       </c>
       <c r="B139" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -3710,7 +3710,7 @@
         <v>154</v>
       </c>
       <c r="B140" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -3718,7 +3718,7 @@
         <v>155</v>
       </c>
       <c r="B141" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -3726,7 +3726,7 @@
         <v>156</v>
       </c>
       <c r="B142" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -3734,7 +3734,7 @@
         <v>157</v>
       </c>
       <c r="B143" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -3742,7 +3742,7 @@
         <v>158</v>
       </c>
       <c r="B144" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -3750,7 +3750,7 @@
         <v>159</v>
       </c>
       <c r="B145" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -3758,7 +3758,7 @@
         <v>160</v>
       </c>
       <c r="B146" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -3766,7 +3766,7 @@
         <v>161</v>
       </c>
       <c r="B147" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -3774,7 +3774,7 @@
         <v>162</v>
       </c>
       <c r="B148" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -3782,7 +3782,7 @@
         <v>163</v>
       </c>
       <c r="B149" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -3790,7 +3790,7 @@
         <v>164</v>
       </c>
       <c r="B150" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -3798,7 +3798,7 @@
         <v>165</v>
       </c>
       <c r="B151" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -3806,7 +3806,7 @@
         <v>166</v>
       </c>
       <c r="B152" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -3814,7 +3814,7 @@
         <v>167</v>
       </c>
       <c r="B153" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -3822,7 +3822,7 @@
         <v>168</v>
       </c>
       <c r="B154" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -3830,7 +3830,7 @@
         <v>169</v>
       </c>
       <c r="B155" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -3838,7 +3838,7 @@
         <v>170</v>
       </c>
       <c r="B156" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -3846,7 +3846,7 @@
         <v>171</v>
       </c>
       <c r="B157" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -3854,7 +3854,7 @@
         <v>172</v>
       </c>
       <c r="B158" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -3862,7 +3862,7 @@
         <v>173</v>
       </c>
       <c r="B159" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -3870,7 +3870,7 @@
         <v>174</v>
       </c>
       <c r="B160" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -3878,7 +3878,7 @@
         <v>175</v>
       </c>
       <c r="B161" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -3886,7 +3886,7 @@
         <v>176</v>
       </c>
       <c r="B162" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -3894,7 +3894,7 @@
         <v>177</v>
       </c>
       <c r="B163" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -3902,7 +3902,7 @@
         <v>178</v>
       </c>
       <c r="B164" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -3910,7 +3910,7 @@
         <v>179</v>
       </c>
       <c r="B165" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -3926,7 +3926,7 @@
         <v>181</v>
       </c>
       <c r="B167" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -3934,7 +3934,7 @@
         <v>182</v>
       </c>
       <c r="B168" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -3942,7 +3942,7 @@
         <v>183</v>
       </c>
       <c r="B169" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -3950,7 +3950,7 @@
         <v>184</v>
       </c>
       <c r="B170" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -3958,7 +3958,7 @@
         <v>185</v>
       </c>
       <c r="B171" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -3966,7 +3966,7 @@
         <v>186</v>
       </c>
       <c r="B172" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -3974,7 +3974,7 @@
         <v>187</v>
       </c>
       <c r="B173" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -3982,7 +3982,7 @@
         <v>188</v>
       </c>
       <c r="B174" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -3990,7 +3990,7 @@
         <v>189</v>
       </c>
       <c r="B175" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -3998,7 +3998,7 @@
         <v>190</v>
       </c>
       <c r="B176" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -4006,7 +4006,7 @@
         <v>191</v>
       </c>
       <c r="B177" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -4014,7 +4014,7 @@
         <v>192</v>
       </c>
       <c r="B178" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -4022,7 +4022,7 @@
         <v>193</v>
       </c>
       <c r="B179" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -4030,7 +4030,7 @@
         <v>194</v>
       </c>
       <c r="B180" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -4038,7 +4038,7 @@
         <v>195</v>
       </c>
       <c r="B181" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -4046,7 +4046,7 @@
         <v>196</v>
       </c>
       <c r="B182" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -4054,7 +4054,7 @@
         <v>197</v>
       </c>
       <c r="B183" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -4062,7 +4062,7 @@
         <v>198</v>
       </c>
       <c r="B184" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -4070,7 +4070,7 @@
         <v>199</v>
       </c>
       <c r="B185" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -4078,7 +4078,7 @@
         <v>200</v>
       </c>
       <c r="B186" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -4086,7 +4086,7 @@
         <v>201</v>
       </c>
       <c r="B187" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -4094,7 +4094,7 @@
         <v>202</v>
       </c>
       <c r="B188" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -4102,7 +4102,7 @@
         <v>203</v>
       </c>
       <c r="B189" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -4110,7 +4110,7 @@
         <v>204</v>
       </c>
       <c r="B190" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -4118,7 +4118,7 @@
         <v>205</v>
       </c>
       <c r="B191" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -4126,7 +4126,7 @@
         <v>206</v>
       </c>
       <c r="B192" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -4134,7 +4134,7 @@
         <v>207</v>
       </c>
       <c r="B193" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -4142,7 +4142,7 @@
         <v>208</v>
       </c>
       <c r="B194" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -4150,7 +4150,7 @@
         <v>209</v>
       </c>
       <c r="B195" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -4158,7 +4158,7 @@
         <v>210</v>
       </c>
       <c r="B196" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -4198,7 +4198,7 @@
         <v>214</v>
       </c>
       <c r="B201" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -4206,7 +4206,7 @@
         <v>215</v>
       </c>
       <c r="B202" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -4214,7 +4214,7 @@
         <v>216</v>
       </c>
       <c r="B203" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -4222,7 +4222,7 @@
         <v>217</v>
       </c>
       <c r="B204" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -4230,7 +4230,7 @@
         <v>218</v>
       </c>
       <c r="B205" t="s">
-        <v>486</v>
+        <v>741</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -4238,7 +4238,7 @@
         <v>219</v>
       </c>
       <c r="B206" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -4246,7 +4246,7 @@
         <v>220</v>
       </c>
       <c r="B207" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -4254,7 +4254,7 @@
         <v>221</v>
       </c>
       <c r="B208" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
@@ -4262,7 +4262,7 @@
         <v>222</v>
       </c>
       <c r="B209" t="s">
-        <v>488</v>
+        <v>739</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -4270,7 +4270,7 @@
         <v>223</v>
       </c>
       <c r="B210" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -4278,7 +4278,7 @@
         <v>224</v>
       </c>
       <c r="B211" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -4286,7 +4286,7 @@
         <v>225</v>
       </c>
       <c r="B212" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
@@ -4294,7 +4294,7 @@
         <v>226</v>
       </c>
       <c r="B213" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
@@ -4302,7 +4302,7 @@
         <v>227</v>
       </c>
       <c r="B214" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
@@ -4310,7 +4310,7 @@
         <v>228</v>
       </c>
       <c r="B215" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
@@ -4318,7 +4318,7 @@
         <v>229</v>
       </c>
       <c r="B216" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
@@ -4326,7 +4326,7 @@
         <v>230</v>
       </c>
       <c r="B217" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
@@ -4334,7 +4334,7 @@
         <v>231</v>
       </c>
       <c r="B218" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
@@ -4342,7 +4342,7 @@
         <v>232</v>
       </c>
       <c r="B219" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -4350,7 +4350,7 @@
         <v>233</v>
       </c>
       <c r="B220" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -4358,7 +4358,7 @@
         <v>234</v>
       </c>
       <c r="B221" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
@@ -4366,7 +4366,7 @@
         <v>235</v>
       </c>
       <c r="B222" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
@@ -4374,7 +4374,7 @@
         <v>236</v>
       </c>
       <c r="B223" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
@@ -4382,7 +4382,7 @@
         <v>237</v>
       </c>
       <c r="B224" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
@@ -4390,7 +4390,7 @@
         <v>238</v>
       </c>
       <c r="B225" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -4398,7 +4398,7 @@
         <v>239</v>
       </c>
       <c r="B226" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
@@ -4406,7 +4406,7 @@
         <v>240</v>
       </c>
       <c r="B227" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
@@ -4414,7 +4414,7 @@
         <v>241</v>
       </c>
       <c r="B228" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -4430,7 +4430,7 @@
         <v>243</v>
       </c>
       <c r="B230" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
@@ -4438,7 +4438,7 @@
         <v>244</v>
       </c>
       <c r="B231" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -4446,7 +4446,7 @@
         <v>245</v>
       </c>
       <c r="B232" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
@@ -4454,7 +4454,7 @@
         <v>246</v>
       </c>
       <c r="B233" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
@@ -4462,7 +4462,7 @@
         <v>247</v>
       </c>
       <c r="B234" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -4470,7 +4470,7 @@
         <v>248</v>
       </c>
       <c r="B235" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
@@ -4478,7 +4478,7 @@
         <v>249</v>
       </c>
       <c r="B236" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
@@ -4486,7 +4486,7 @@
         <v>250</v>
       </c>
       <c r="B237" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -4494,7 +4494,7 @@
         <v>251</v>
       </c>
       <c r="B238" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
@@ -4502,7 +4502,7 @@
         <v>252</v>
       </c>
       <c r="B239" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
@@ -4510,7 +4510,7 @@
         <v>253</v>
       </c>
       <c r="B240" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
@@ -4518,7 +4518,7 @@
         <v>254</v>
       </c>
       <c r="B241" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
@@ -4526,7 +4526,7 @@
         <v>255</v>
       </c>
       <c r="B242" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
@@ -4534,7 +4534,7 @@
         <v>256</v>
       </c>
       <c r="B243" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -4542,7 +4542,7 @@
         <v>257</v>
       </c>
       <c r="B244" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
@@ -4550,7 +4550,7 @@
         <v>258</v>
       </c>
       <c r="B245" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
@@ -4558,7 +4558,7 @@
         <v>259</v>
       </c>
       <c r="B246" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -4566,7 +4566,7 @@
         <v>260</v>
       </c>
       <c r="B247" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
@@ -4574,7 +4574,7 @@
         <v>261</v>
       </c>
       <c r="B248" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
@@ -4582,7 +4582,7 @@
         <v>262</v>
       </c>
       <c r="B249" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
@@ -4590,7 +4590,7 @@
         <v>263</v>
       </c>
       <c r="B250" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
@@ -4598,7 +4598,7 @@
         <v>264</v>
       </c>
       <c r="B251" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
@@ -4606,7 +4606,7 @@
         <v>265</v>
       </c>
       <c r="B252" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
@@ -4614,7 +4614,7 @@
         <v>266</v>
       </c>
       <c r="B253" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
@@ -4622,7 +4622,7 @@
         <v>267</v>
       </c>
       <c r="B254" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
@@ -4630,7 +4630,7 @@
         <v>268</v>
       </c>
       <c r="B255" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
@@ -4638,7 +4638,7 @@
         <v>269</v>
       </c>
       <c r="B256" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
@@ -4646,7 +4646,7 @@
         <v>270</v>
       </c>
       <c r="B257" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
@@ -4654,7 +4654,7 @@
         <v>271</v>
       </c>
       <c r="B258" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
@@ -4662,7 +4662,7 @@
         <v>272</v>
       </c>
       <c r="B259" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
@@ -4670,7 +4670,7 @@
         <v>273</v>
       </c>
       <c r="B260" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
@@ -4678,7 +4678,7 @@
         <v>274</v>
       </c>
       <c r="B261" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
@@ -4686,7 +4686,7 @@
         <v>275</v>
       </c>
       <c r="B262" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
@@ -4694,7 +4694,7 @@
         <v>276</v>
       </c>
       <c r="B263" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
@@ -4702,7 +4702,7 @@
         <v>277</v>
       </c>
       <c r="B264" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
@@ -4710,7 +4710,7 @@
         <v>278</v>
       </c>
       <c r="B265" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
@@ -4718,7 +4718,7 @@
         <v>279</v>
       </c>
       <c r="B266" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
@@ -4726,7 +4726,7 @@
         <v>280</v>
       </c>
       <c r="B267" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
@@ -4734,7 +4734,7 @@
         <v>281</v>
       </c>
       <c r="B268" t="s">
-        <v>685</v>
+        <v>679</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
@@ -4742,7 +4742,7 @@
         <v>282</v>
       </c>
       <c r="B269" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
@@ -4750,7 +4750,7 @@
         <v>283</v>
       </c>
       <c r="B270" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
@@ -4758,7 +4758,7 @@
         <v>284</v>
       </c>
       <c r="B271" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
@@ -4766,7 +4766,7 @@
         <v>285</v>
       </c>
       <c r="B272" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
@@ -4774,7 +4774,7 @@
         <v>286</v>
       </c>
       <c r="B273" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
@@ -4782,7 +4782,7 @@
         <v>287</v>
       </c>
       <c r="B274" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
@@ -4790,7 +4790,7 @@
         <v>288</v>
       </c>
       <c r="B275" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
@@ -4798,7 +4798,7 @@
         <v>289</v>
       </c>
       <c r="B276" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
@@ -4806,7 +4806,7 @@
         <v>290</v>
       </c>
       <c r="B277" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
@@ -4822,7 +4822,7 @@
         <v>292</v>
       </c>
       <c r="B279" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
@@ -4838,7 +4838,7 @@
         <v>294</v>
       </c>
       <c r="B281" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
@@ -4846,7 +4846,7 @@
         <v>295</v>
       </c>
       <c r="B282" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
@@ -4854,7 +4854,7 @@
         <v>296</v>
       </c>
       <c r="B283" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
@@ -4862,7 +4862,7 @@
         <v>297</v>
       </c>
       <c r="B284" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
@@ -4870,7 +4870,7 @@
         <v>298</v>
       </c>
       <c r="B285" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
@@ -4878,7 +4878,7 @@
         <v>299</v>
       </c>
       <c r="B286" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
@@ -4886,7 +4886,7 @@
         <v>300</v>
       </c>
       <c r="B287" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
@@ -4894,7 +4894,7 @@
         <v>301</v>
       </c>
       <c r="B288" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
@@ -4902,7 +4902,7 @@
         <v>302</v>
       </c>
       <c r="B289" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
@@ -4910,7 +4910,7 @@
         <v>303</v>
       </c>
       <c r="B290" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
@@ -4918,7 +4918,7 @@
         <v>304</v>
       </c>
       <c r="B291" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
@@ -4926,7 +4926,7 @@
         <v>305</v>
       </c>
       <c r="B292" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
@@ -4934,7 +4934,7 @@
         <v>306</v>
       </c>
       <c r="B293" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
@@ -4942,7 +4942,7 @@
         <v>307</v>
       </c>
       <c r="B294" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
@@ -4950,7 +4950,7 @@
         <v>308</v>
       </c>
       <c r="B295" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
@@ -4958,7 +4958,7 @@
         <v>309</v>
       </c>
       <c r="B296" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
@@ -4966,7 +4966,7 @@
         <v>310</v>
       </c>
       <c r="B297" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
@@ -4974,7 +4974,7 @@
         <v>311</v>
       </c>
       <c r="B298" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
@@ -4982,7 +4982,7 @@
         <v>312</v>
       </c>
       <c r="B299" t="s">
-        <v>701</v>
+        <v>695</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
@@ -4990,7 +4990,7 @@
         <v>313</v>
       </c>
       <c r="B300" t="s">
-        <v>702</v>
+        <v>696</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
@@ -4998,7 +4998,7 @@
         <v>314</v>
       </c>
       <c r="B301" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
@@ -5006,7 +5006,7 @@
         <v>315</v>
       </c>
       <c r="B302" t="s">
-        <v>703</v>
+        <v>697</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
@@ -5014,7 +5014,7 @@
         <v>316</v>
       </c>
       <c r="B303" t="s">
-        <v>704</v>
+        <v>698</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
@@ -5022,7 +5022,7 @@
         <v>317</v>
       </c>
       <c r="B304" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
@@ -5030,7 +5030,7 @@
         <v>318</v>
       </c>
       <c r="B305" t="s">
-        <v>705</v>
+        <v>699</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
@@ -5038,7 +5038,7 @@
         <v>319</v>
       </c>
       <c r="B306" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
@@ -5046,7 +5046,7 @@
         <v>320</v>
       </c>
       <c r="B307" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
@@ -5054,7 +5054,7 @@
         <v>321</v>
       </c>
       <c r="B308" t="s">
-        <v>706</v>
+        <v>700</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
@@ -5062,7 +5062,7 @@
         <v>322</v>
       </c>
       <c r="B309" t="s">
-        <v>707</v>
+        <v>701</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
@@ -5070,7 +5070,7 @@
         <v>323</v>
       </c>
       <c r="B310" t="s">
-        <v>708</v>
+        <v>702</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
@@ -5078,7 +5078,7 @@
         <v>324</v>
       </c>
       <c r="B311" t="s">
-        <v>709</v>
+        <v>703</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
@@ -5086,7 +5086,7 @@
         <v>325</v>
       </c>
       <c r="B312" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
@@ -5094,7 +5094,7 @@
         <v>326</v>
       </c>
       <c r="B313" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
@@ -5102,7 +5102,7 @@
         <v>327</v>
       </c>
       <c r="B314" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
@@ -5110,7 +5110,7 @@
         <v>328</v>
       </c>
       <c r="B315" t="s">
-        <v>711</v>
+        <v>705</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
@@ -5118,7 +5118,7 @@
         <v>329</v>
       </c>
       <c r="B316" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
@@ -5126,7 +5126,7 @@
         <v>330</v>
       </c>
       <c r="B317" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
@@ -5134,7 +5134,7 @@
         <v>331</v>
       </c>
       <c r="B318" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
@@ -5142,7 +5142,7 @@
         <v>332</v>
       </c>
       <c r="B319" t="s">
-        <v>713</v>
+        <v>707</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
@@ -5150,7 +5150,7 @@
         <v>333</v>
       </c>
       <c r="B320" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
@@ -5158,7 +5158,7 @@
         <v>334</v>
       </c>
       <c r="B321" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
@@ -5166,7 +5166,7 @@
         <v>335</v>
       </c>
       <c r="B322" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
@@ -5174,7 +5174,7 @@
         <v>336</v>
       </c>
       <c r="B323" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
@@ -5182,7 +5182,7 @@
         <v>337</v>
       </c>
       <c r="B324" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
@@ -5190,7 +5190,7 @@
         <v>338</v>
       </c>
       <c r="B325" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
@@ -5198,7 +5198,7 @@
         <v>339</v>
       </c>
       <c r="B326" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
@@ -5206,7 +5206,7 @@
         <v>340</v>
       </c>
       <c r="B327" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
@@ -5214,7 +5214,7 @@
         <v>341</v>
       </c>
       <c r="B328" t="s">
-        <v>715</v>
+        <v>709</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
@@ -5222,7 +5222,7 @@
         <v>342</v>
       </c>
       <c r="B329" t="s">
-        <v>716</v>
+        <v>710</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
@@ -5230,7 +5230,7 @@
         <v>343</v>
       </c>
       <c r="B330" t="s">
-        <v>717</v>
+        <v>711</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
@@ -5238,7 +5238,7 @@
         <v>344</v>
       </c>
       <c r="B331" t="s">
-        <v>718</v>
+        <v>712</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
@@ -5246,7 +5246,7 @@
         <v>345</v>
       </c>
       <c r="B332" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
@@ -5254,7 +5254,7 @@
         <v>346</v>
       </c>
       <c r="B333" t="s">
-        <v>719</v>
+        <v>713</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
@@ -5262,7 +5262,7 @@
         <v>347</v>
       </c>
       <c r="B334" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
@@ -5270,7 +5270,7 @@
         <v>348</v>
       </c>
       <c r="B335" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
@@ -5278,7 +5278,7 @@
         <v>349</v>
       </c>
       <c r="B336" t="s">
-        <v>720</v>
+        <v>714</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
@@ -5286,7 +5286,7 @@
         <v>350</v>
       </c>
       <c r="B337" t="s">
-        <v>721</v>
+        <v>715</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
@@ -5294,7 +5294,7 @@
         <v>351</v>
       </c>
       <c r="B338" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
@@ -5302,7 +5302,7 @@
         <v>352</v>
       </c>
       <c r="B339" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
@@ -5310,7 +5310,7 @@
         <v>353</v>
       </c>
       <c r="B340" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
@@ -5318,7 +5318,7 @@
         <v>354</v>
       </c>
       <c r="B341" t="s">
-        <v>724</v>
+        <v>718</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
@@ -5326,7 +5326,7 @@
         <v>355</v>
       </c>
       <c r="B342" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
@@ -5334,7 +5334,7 @@
         <v>356</v>
       </c>
       <c r="B343" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
@@ -5342,7 +5342,7 @@
         <v>357</v>
       </c>
       <c r="B344" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
@@ -5350,7 +5350,7 @@
         <v>358</v>
       </c>
       <c r="B345" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
@@ -5358,7 +5358,7 @@
         <v>359</v>
       </c>
       <c r="B346" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
@@ -5366,7 +5366,7 @@
         <v>360</v>
       </c>
       <c r="B347" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
@@ -5382,7 +5382,7 @@
         <v>362</v>
       </c>
       <c r="B349" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
@@ -5390,7 +5390,7 @@
         <v>363</v>
       </c>
       <c r="B350" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
@@ -5398,7 +5398,7 @@
         <v>364</v>
       </c>
       <c r="B351" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
@@ -5406,7 +5406,7 @@
         <v>365</v>
       </c>
       <c r="B352" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
@@ -5414,7 +5414,7 @@
         <v>366</v>
       </c>
       <c r="B353" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
@@ -5422,7 +5422,7 @@
         <v>367</v>
       </c>
       <c r="B354" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
@@ -5430,7 +5430,7 @@
         <v>368</v>
       </c>
       <c r="B355" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
@@ -5438,7 +5438,7 @@
         <v>369</v>
       </c>
       <c r="B356" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
@@ -5446,7 +5446,7 @@
         <v>370</v>
       </c>
       <c r="B357" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
@@ -5454,7 +5454,7 @@
         <v>371</v>
       </c>
       <c r="B358" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
@@ -5462,7 +5462,7 @@
         <v>372</v>
       </c>
       <c r="B359" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
@@ -5470,7 +5470,7 @@
         <v>373</v>
       </c>
       <c r="B360" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
@@ -5478,7 +5478,7 @@
         <v>374</v>
       </c>
       <c r="B361" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
@@ -5486,7 +5486,7 @@
         <v>375</v>
       </c>
       <c r="B362" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
@@ -5494,7 +5494,7 @@
         <v>376</v>
       </c>
       <c r="B363" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
@@ -5502,7 +5502,7 @@
         <v>377</v>
       </c>
       <c r="B364" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
@@ -5510,7 +5510,7 @@
         <v>378</v>
       </c>
       <c r="B365" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
@@ -5518,7 +5518,7 @@
         <v>379</v>
       </c>
       <c r="B366" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
@@ -5526,7 +5526,7 @@
         <v>380</v>
       </c>
       <c r="B367" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
@@ -5534,7 +5534,7 @@
         <v>381</v>
       </c>
       <c r="B368" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
@@ -5542,7 +5542,7 @@
         <v>261</v>
       </c>
       <c r="B369" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
@@ -5550,7 +5550,7 @@
         <v>382</v>
       </c>
       <c r="B370" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
@@ -5558,7 +5558,7 @@
         <v>383</v>
       </c>
       <c r="B371" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
@@ -5566,7 +5566,7 @@
         <v>384</v>
       </c>
       <c r="B372" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
     </row>
   </sheetData>

</xml_diff>